<commit_message>
add data for train bot
</commit_message>
<xml_diff>
--- a/chat_bot/data/response_law.xlsx
+++ b/chat_bot/data/response_law.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chatbot_law\chat_bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>tag</t>
   </si>
@@ -107,54 +107,42 @@
     <t>quetions-law</t>
   </si>
   <si>
-    <t>กฎหมายภาษี เป็นกฎหมายที่บัญญัติขึ้นภายใต้รัฐธรรมนูญ โดยมีจุดประสงค์เพื่อกำหนดควบคุมอัตราการแลกเปลี่ยนเงินในประเทศและเป็นกฎหมายที่ให้อำนาจแก่รัฐในการจัดเก็บภาษีจากราษฎร เพื่อนำไปใช้เป็นประโยชน์ต่อสังคมโดยรวมและผลักดันการพัฒนาเศรษฐกิจของประเทศ ครับ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">กฎหมายภาษี เป็นกฎหมายที่บัญญัติขึ้นภายใต้รัฐธรรมนูญ </t>
-  </si>
-  <si>
-    <t>กฎหมายภาษีมีจุดประสงค์เพื่อกำหนดควบคุมอัตราการแลกเปลี่ยนเงินในประเทศและเป็นกฎหมายที่ให้อำนาจแก่รัฐในการจัดเก็บภาษีจากราษฎร</t>
-  </si>
-  <si>
-    <t>กฎหมายภาษี เป็นกฎหมายที่บัญญัติขึ้นภายใต้รัฐธรรมนูญ โดยมีจุดประสงค์เพื่อนำไปใช้เป็นประโยชน์ต่อสังคมโดยรวมและผลักดันการพัฒนาเศรษฐกิจของประเทศ ครับ</t>
-  </si>
-  <si>
-    <t>เป็นกฎหมายที่บัญญัติขึ้นภายใต้รัฐธรรมนูญ เพื่อนำไปใช้เป็นประโยชน์ต่อสังคมโดยรวมและผลักดันการพัฒนาเศรษฐกิจของประเทศ ครับ</t>
-  </si>
-  <si>
-    <t>เป็นกฎหมายที่บัญญัติขึ้นภายใต้รัฐธรรมนูญ โดยมีจุดประสงค์เพื่อกำหนดควบคุมอัตราการแลกเปลี่ยนเงินในประเทศและเป็นกฎหมายที่ให้อำนาจแก่รัฐในการจัดเก็บภาษีจากราษฎร เพื่อนำไปใช้เป็นประโยชน์ต่อสังคมโดยรวมและผลักดันการพัฒนาเศรษฐกิจของประเทศ ครับ</t>
-  </si>
-  <si>
     <t>law-type</t>
   </si>
   <si>
-    <t>ภาษี สามารแบ่งออกเป็น 5 ประเภทด้วยกันครับ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ภาษี สามารแบ่งออกเป็น 5 ประเภทด้วยกันครับ
+    <t>law-claim</t>
+  </si>
+  <si>
+    <t>law-taxation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not-pay </t>
+  </si>
+  <si>
+    <t>ภาษี สามารแบ่งออกเป็น 5 ประเภทด้วยกันครับ
  1.ภาษีบุคคลธรรมดา(PIT)
  2.ภาษีเงินได้นิติบุคคล 
  3.ภาษีมูลค่าเพิ่ม(VAT) 
  4.ภาษีธุรกิจเฉพาะ(SBT)
- 5.อากรแสตมป์(SD)
-</t>
-  </si>
-  <si>
-    <t>ภาษีแบ่งออกเป็น 5 ประเภทค่ะ</t>
-  </si>
-  <si>
-    <t>ภาษีแบ่งเป็น 5 ประเภท</t>
-  </si>
-  <si>
-    <t>law-claim</t>
+ 5.อากรแสตมป์(SD)</t>
+  </si>
+  <si>
+    <t>หากไม่เสียภาษีตามกฎหมายที่กำหนด ตามบทบัญญัติแห่งประมวลกฎหมายรัษฎากร โดยปกติประชาชนทุกคนไม่ว่าจะบุคคลใดจะต้องมีหน้าที่เสียภาษีตามข้อบังคับของกฎหมายรัฐธรรมนูญ และจำเป็นที่จะต้องมีการยื่นแบบการเสียภาษี เพื่อให้ทางรัฐบาลได้รู้ว่าบุคคลมีความบริสุทธิ์ใจที่จะไม่หลีกเลี่ยงการเสียภาษี หากผู้ใดไม่เสียภาษีตามที่กฎหมายกำหนดจะต้องได้รับโทษตามประมวลกฎหมายรัษฎากรและต้องรับผิดทางแพ่งและทางอาญาด้วย</t>
+  </si>
+  <si>
+    <t>กฎหมายภาษี เป็นกฎหมายที่บัญญัติขึ้นภายใต้รัฐธรรมนูญ โดยมีจุดประสงค์เพื่อกำหนดควบคุมอัตราการแลกเปลี่ยนเงินในประเทศและเป็นกฎหมายที่ให้อำนาจแก่รัฐในการจัดเก็บภาษีจากราษฎร เพื่อนำไปใช้เป็นประโยชน์ต่อสังคมโดยรวมและผลักดันการพัฒนาเศรษฐกิจของประเทศครับ</t>
   </si>
   <si>
     <t xml:space="preserve">1.การผ่อนชำระภาษี
-  2.การยื่นอุทธรณ์คัดค้านการประเมินภาษี 
-  3.ขอทุเลาการชำระภาษีอากรโดยจัดให้มีหลักประกันการชำระหนี้ภาษีอากรค้าง 
-  4.ของดหรือลดเบี้ยปรับและเงินเพิ่มภาษีอากร 
-  5.ขอคัดเอกสารหรือขอสำเนาเอกสาร 
-</t>
+2.การยื่นอุทธรณ์คัดค้านการประเมินภาษี 
+3.ขอทุเลาการชำระภาษีอากรโดยจัดให้มีหลักประกันการชำระหนี้ภาษีอากรค้าง 
+4.ของดหรือลดเบี้ยปรับและเงินเพิ่มภาษีอากร 
+5.ขอคัดเอกสารหรือขอสำเนาเอกสาร </t>
+  </si>
+  <si>
+    <t>หน่วยงานของรัฐสามารถจัดเก็บภาษีอากร แบ่งเป็น 2 ทาง ดังนี้
+ภาษีทางตรง ได้แก่  ภาษีเงินได้บุคคลธรรมดา ภาษีเงินได้นิติบุคคล 
+ภาษีทางอ้อม ได้แก่ ภาษีมูลค่าเพิ่ม ภาษีธุรกิจเฉพาะ</t>
   </si>
 </sst>
 </file>
@@ -503,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="106" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -568,7 +556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="51">
+    <row r="8" spans="1:2" ht="25.5">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -624,7 +612,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="38.25">
+    <row r="15" spans="1:2" ht="28.5">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -640,7 +628,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="51">
+    <row r="17" spans="1:2" ht="28.5">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -656,7 +644,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="38.25">
+    <row r="19" spans="1:2" ht="28.5">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -664,7 +652,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="38.25">
+    <row r="20" spans="1:2" ht="28.5">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -672,93 +660,67 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="409.5">
+    <row r="21" spans="1:2" ht="89.25">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="76.5">
       <c r="A22" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="76.5">
+      <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="216.75">
-      <c r="A23" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="B23" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="76.5">
+      <c r="A24" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="267.75">
-      <c r="A24" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="B24" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="127.5">
+      <c r="A25" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="229.5">
-      <c r="A25" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="B25" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="409.5">
-      <c r="A26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="63.75">
-      <c r="A27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="280.5">
-      <c r="A28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="38.25">
-      <c r="A29" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>36</v>
-      </c>
+    <row r="26" spans="1:2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="89.25">
-      <c r="A31" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add data and response for test bot
</commit_message>
<xml_diff>
--- a/chat_bot/data/response_law.xlsx
+++ b/chat_bot/data/response_law.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>tag</t>
   </si>
@@ -143,6 +143,32 @@
     <t>หน่วยงานของรัฐสามารถจัดเก็บภาษีอากร แบ่งเป็น 2 ทาง ดังนี้
 ภาษีทางตรง ได้แก่  ภาษีเงินได้บุคคลธรรมดา ภาษีเงินได้นิติบุคคล 
 ภาษีทางอ้อม ได้แก่ ภาษีมูลค่าเพิ่ม ภาษีธุรกิจเฉพาะ</t>
+  </si>
+  <si>
+    <t>law-why</t>
+  </si>
+  <si>
+    <t>เพื่อเป็นเครื่องมือส่งเสริมความเจริญเติบโตทางเศรษฐกิจ
+ -เพื่อเป็นเครื่องมือในการควบคุมการบริโภคของประชาชนและบำรุงสาธารณูปโภคเละบริการสาธารณะ
+ -เพื่อเป็นเครื่องมือในการกระจายรายได้แก่ให้ประชาชนและเป็นการรักษาเสถียรภาพในทางเศรษฐกิจของประเทศ</t>
+  </si>
+  <si>
+    <t>law-calculate</t>
+  </si>
+  <si>
+    <t>การคำนวณภาษีของบุคคลธรรมดา เงินได้สุทธิซึ่งเป็นฐานภาษีสำหรับคำนวณภาษีเงินได้บุคคลธรรมดาซึ่งมาจากเงินได้พึงประเมินที่หักค่าใช้จ่ายและค่าลดหย่อนเรียบร้อยแล้ว (ค่าใช้จ่าย-ค่าลดหย่อน=เงินได้สุทธิ)</t>
+  </si>
+  <si>
+    <t>law-time</t>
+  </si>
+  <si>
+    <t>กฎหมายกำหนดให้บุคคลต้องทำการยื่นเสียภาษีในช่วง 1 มกราคม - 31 มีนาคม ของทุกปี</t>
+  </si>
+  <si>
+    <t>law-salary</t>
+  </si>
+  <si>
+    <t>หากมีเงินเดือนหรือมีรายได้จากหลายทางเกิน 10,000 บาท/เดือน (120,000 บาท/ปี) ต้องยื่นภาษีทุกคน</t>
   </si>
 </sst>
 </file>
@@ -491,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="106" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="106" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -700,20 +726,37 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="3"/>
+    <row r="26" spans="1:2" ht="102">
+      <c r="A26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="63.75">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="25.5">
+      <c r="A28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="38.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="30" spans="1:2">
       <c r="B30" s="3"/>

</xml_diff>

<commit_message>
add response topic law-place
</commit_message>
<xml_diff>
--- a/chat_bot/data/response_law.xlsx
+++ b/chat_bot/data/response_law.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>tag</t>
   </si>
@@ -169,6 +169,14 @@
   </si>
   <si>
     <t>หากมีเงินเดือนหรือมีรายได้จากหลายทางเกิน 10,000 บาท/เดือน (120,000 บาท/ปี) ต้องยื่นภาษีทุกคน</t>
+  </si>
+  <si>
+    <t>law-place</t>
+  </si>
+  <si>
+    <t>1.สำนักงานสรรพากรทุกสาขาทุกเเห่ง 
+2.ไปรษณีย์ เเบบลงทะเบียน 
+3.ช่องทางออนไลน์ ผ่านเว็บไซต์ของกรมสรรพากร</t>
   </si>
 </sst>
 </file>
@@ -517,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="106" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -752,14 +760,19 @@
     </row>
     <row r="29" spans="1:2" ht="38.25">
       <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="38.25">
+      <c r="A30" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="4"/>

</xml_diff>

<commit_message>
add text in response_law.xlsx
</commit_message>
<xml_diff>
--- a/chat_bot/data/response_law.xlsx
+++ b/chat_bot/data/response_law.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>tag</t>
   </si>
@@ -143,6 +143,40 @@
     <t>หน่วยงานของรัฐสามารถจัดเก็บภาษีอากร แบ่งเป็น 2 ทาง ดังนี้
 ภาษีทางตรง ได้แก่  ภาษีเงินได้บุคคลธรรมดา ภาษีเงินได้นิติบุคคล 
 ภาษีทางอ้อม ได้แก่ ภาษีมูลค่าเพิ่ม ภาษีธุรกิจเฉพาะ</t>
+  </si>
+  <si>
+    <t>law-why</t>
+  </si>
+  <si>
+    <t>เพื่อเป็นเครื่องมือส่งเสริมความเจริญเติบโตทางเศรษฐกิจ
+ -เพื่อเป็นเครื่องมือในการควบคุมการบริโภคของประชาชนและบำรุงสาธารณูปโภคเละบริการสาธารณะ
+ -เพื่อเป็นเครื่องมือในการกระจายรายได้แก่ให้ประชาชนและเป็นการรักษาเสถียรภาพในทางเศรษฐกิจของประเทศ</t>
+  </si>
+  <si>
+    <t>law-calculate</t>
+  </si>
+  <si>
+    <t>การคำนวณภาษีของบุคคลธรรมดา เงินได้สุทธิซึ่งเป็นฐานภาษีสำหรับคำนวณภาษีเงินได้บุคคลธรรมดาซึ่งมาจากเงินได้พึงประเมินที่หักค่าใช้จ่ายและค่าลดหย่อนเรียบร้อยแล้ว (ค่าใช้จ่าย-ค่าลดหย่อน=เงินได้สุทธิ)</t>
+  </si>
+  <si>
+    <t>law-time</t>
+  </si>
+  <si>
+    <t>กฎหมายกำหนดให้บุคคลต้องทำการยื่นเสียภาษีในช่วง 1 มกราคม - 31 มีนาคม ของทุกปี</t>
+  </si>
+  <si>
+    <t>law-salary</t>
+  </si>
+  <si>
+    <t>หากมีเงินเดือนหรือมีรายได้จากหลายทางเกิน 10,000 บาท/เดือน (120,000 บาท/ปี) ต้องยื่นภาษีทุกคน</t>
+  </si>
+  <si>
+    <t>law-place</t>
+  </si>
+  <si>
+    <t>1.สำนักงานสรรพากรทุกสาขาทุกเเห่ง 
+2.ไปรษณีย์ เเบบลงทะเบียน 
+3.ช่องทางออนไลน์ ผ่านเว็บไซต์ของกรมสรรพากร</t>
   </si>
 </sst>
 </file>
@@ -491,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="106" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -700,23 +734,45 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="B30" s="3"/>
+    <row r="26" spans="1:2" ht="102">
+      <c r="A26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="63.75">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="25.5">
+      <c r="A28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="38.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="38.25">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="4"/>

</xml_diff>

<commit_message>
add response if bot unknow message
</commit_message>
<xml_diff>
--- a/chat_bot/data/response_law.xlsx
+++ b/chat_bot/data/response_law.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>tag</t>
   </si>
@@ -133,50 +133,64 @@
     <t>กฎหมายภาษี เป็นกฎหมายที่บัญญัติขึ้นภายใต้รัฐธรรมนูญ โดยมีจุดประสงค์เพื่อกำหนดควบคุมอัตราการแลกเปลี่ยนเงินในประเทศและเป็นกฎหมายที่ให้อำนาจแก่รัฐในการจัดเก็บภาษีจากราษฎร เพื่อนำไปใช้เป็นประโยชน์ต่อสังคมโดยรวมและผลักดันการพัฒนาเศรษฐกิจของประเทศครับ</t>
   </si>
   <si>
-    <t xml:space="preserve">1.การผ่อนชำระภาษี
+    <t>หน่วยงานของรัฐสามารถจัดเก็บภาษีอากร แบ่งเป็น 2 ทาง ดังนี้
+ภาษีทางตรง ได้แก่  ภาษีเงินได้บุคคลธรรมดา ภาษีเงินได้นิติบุคคล 
+ภาษีทางอ้อม ได้แก่ ภาษีมูลค่าเพิ่ม ภาษีธุรกิจเฉพาะ</t>
+  </si>
+  <si>
+    <t>law-why</t>
+  </si>
+  <si>
+    <t>เพื่อเป็นเครื่องมือส่งเสริมความเจริญเติบโตทางเศรษฐกิจ
+ -เพื่อเป็นเครื่องมือในการควบคุมการบริโภคของประชาชนและบำรุงสาธารณูปโภคเละบริการสาธารณะ
+ -เพื่อเป็นเครื่องมือในการกระจายรายได้แก่ให้ประชาชนและเป็นการรักษาเสถียรภาพในทางเศรษฐกิจของประเทศ</t>
+  </si>
+  <si>
+    <t>law-calculate</t>
+  </si>
+  <si>
+    <t>การคำนวณภาษีของบุคคลธรรมดา เงินได้สุทธิซึ่งเป็นฐานภาษีสำหรับคำนวณภาษีเงินได้บุคคลธรรมดาซึ่งมาจากเงินได้พึงประเมินที่หักค่าใช้จ่ายและค่าลดหย่อนเรียบร้อยแล้ว (ค่าใช้จ่าย-ค่าลดหย่อน=เงินได้สุทธิ)</t>
+  </si>
+  <si>
+    <t>law-time</t>
+  </si>
+  <si>
+    <t>กฎหมายกำหนดให้บุคคลต้องทำการยื่นเสียภาษีในช่วง 1 มกราคม - 31 มีนาคม ของทุกปี</t>
+  </si>
+  <si>
+    <t>law-salary</t>
+  </si>
+  <si>
+    <t>หากมีเงินเดือนหรือมีรายได้จากหลายทางเกิน 10,000 บาท/เดือน (120,000 บาท/ปี) ต้องยื่นภาษีทุกคน</t>
+  </si>
+  <si>
+    <t>law-place</t>
+  </si>
+  <si>
+    <t>1.สำนักงานสรรพากรทุกสาขาทุกเเห่ง 
+2.ไปรษณีย์ เเบบลงทะเบียน 
+3.ช่องทางออนไลน์ ผ่านเว็บไซต์ของกรมสรรพากร</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ขออภัยค่ะ ระบบอัติโนมัติยังไม่เข้าใจคำถามของคุณ หากต้องการสอบถามข้อมูลด้านใดเกี่ยวกับภาษี สามารถถามคำถามดังต่อไปนี้ได้เลยค่ะ
+1.กฎหมายภาษืคืออะไร
+2.ภาษีมีกี่ประเภท
+3.สิทธิของประชาชนผู้เสียภาษีมีอะไรบ้าง
+4.หน่วยงานของรัฐสามารถจัดเก็บภาษีอากรประเภทไหนได้บ้าง
+5.หากไม่เสียภาษีตามที่กฎหมายกำหนด จะส่งผลอย่างไร
+6.ทำไมหน่วยงานรัฐถึงต้องจัดเก็บภาษี?
+7.ภาษีบุคคลธรรมดาคำนวณจากอะไรและคำนวนอย่างไร
+8.กฎหมายกำหนดให้บุคคลต้องทำการยื่นเสียภาษีในช่วงเดือนใด
+9.ถ้าต้องการที่จะเสียภาษี สามารถยื่นเสียภาษีได้ที่ไหนบ้าง 
+10.บุคคลธรรมดาต้องมีเงินเดือนเท่าไร ถึงต้องยื่นภาษี </t>
+  </si>
+  <si>
+    <t xml:space="preserve">สิทธิของประชาชนผู้เสียภาษีมีดังต่อไปนี้
+1.การผ่อนชำระภาษี
 2.การยื่นอุทธรณ์คัดค้านการประเมินภาษี 
 3.ขอทุเลาการชำระภาษีอากรโดยจัดให้มีหลักประกันการชำระหนี้ภาษีอากรค้าง 
 4.ของดหรือลดเบี้ยปรับและเงินเพิ่มภาษีอากร 
 5.ขอคัดเอกสารหรือขอสำเนาเอกสาร </t>
-  </si>
-  <si>
-    <t>หน่วยงานของรัฐสามารถจัดเก็บภาษีอากร แบ่งเป็น 2 ทาง ดังนี้
-ภาษีทางตรง ได้แก่  ภาษีเงินได้บุคคลธรรมดา ภาษีเงินได้นิติบุคคล 
-ภาษีทางอ้อม ได้แก่ ภาษีมูลค่าเพิ่ม ภาษีธุรกิจเฉพาะ</t>
-  </si>
-  <si>
-    <t>law-why</t>
-  </si>
-  <si>
-    <t>เพื่อเป็นเครื่องมือส่งเสริมความเจริญเติบโตทางเศรษฐกิจ
- -เพื่อเป็นเครื่องมือในการควบคุมการบริโภคของประชาชนและบำรุงสาธารณูปโภคเละบริการสาธารณะ
- -เพื่อเป็นเครื่องมือในการกระจายรายได้แก่ให้ประชาชนและเป็นการรักษาเสถียรภาพในทางเศรษฐกิจของประเทศ</t>
-  </si>
-  <si>
-    <t>law-calculate</t>
-  </si>
-  <si>
-    <t>การคำนวณภาษีของบุคคลธรรมดา เงินได้สุทธิซึ่งเป็นฐานภาษีสำหรับคำนวณภาษีเงินได้บุคคลธรรมดาซึ่งมาจากเงินได้พึงประเมินที่หักค่าใช้จ่ายและค่าลดหย่อนเรียบร้อยแล้ว (ค่าใช้จ่าย-ค่าลดหย่อน=เงินได้สุทธิ)</t>
-  </si>
-  <si>
-    <t>law-time</t>
-  </si>
-  <si>
-    <t>กฎหมายกำหนดให้บุคคลต้องทำการยื่นเสียภาษีในช่วง 1 มกราคม - 31 มีนาคม ของทุกปี</t>
-  </si>
-  <si>
-    <t>law-salary</t>
-  </si>
-  <si>
-    <t>หากมีเงินเดือนหรือมีรายได้จากหลายทางเกิน 10,000 บาท/เดือน (120,000 บาท/ปี) ต้องยื่นภาษีทุกคน</t>
-  </si>
-  <si>
-    <t>law-place</t>
-  </si>
-  <si>
-    <t>1.สำนักงานสรรพากรทุกสาขาทุกเเห่ง 
-2.ไปรษณีย์ เเบบลงทะเบียน 
-3.ช่องทางออนไลน์ ผ่านเว็บไซต์ของกรมสรรพากร</t>
   </si>
 </sst>
 </file>
@@ -525,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -710,12 +724,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="76.5">
+    <row r="23" spans="1:2" ht="89.25">
       <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="76.5">
@@ -723,7 +737,7 @@
         <v>29</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="127.5">
@@ -736,47 +750,51 @@
     </row>
     <row r="26" spans="1:2" ht="102">
       <c r="A26" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="63.75">
       <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="25.5">
       <c r="A28" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="38.25">
       <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="38.25">
       <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="3"/>
+    </row>
+    <row r="31" spans="1:2" ht="242.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add response and question about place to pay taxes
</commit_message>
<xml_diff>
--- a/chat_bot/data/response_law.xlsx
+++ b/chat_bot/data/response_law.xlsx
@@ -167,11 +167,6 @@
     <t>law-place</t>
   </si>
   <si>
-    <t>1.สำนักงานสรรพากรทุกสาขาทุกเเห่ง 
-2.ไปรษณีย์ เเบบลงทะเบียน 
-3.ช่องทางออนไลน์ ผ่านเว็บไซต์ของกรมสรรพากร</t>
-  </si>
-  <si>
     <t xml:space="preserve">ขออภัยค่ะ ระบบอัติโนมัติยังไม่เข้าใจคำถามของคุณ หากต้องการสอบถามข้อมูลด้านใดเกี่ยวกับภาษี สามารถถามคำถามดังต่อไปนี้ได้เลยค่ะ
 1.กฎหมายภาษืคืออะไร
 2.ภาษีมีกี่ประเภท
@@ -191,6 +186,12 @@
 3.ขอทุเลาการชำระภาษีอากรโดยจัดให้มีหลักประกันการชำระหนี้ภาษีอากรค้าง 
 4.ของดหรือลดเบี้ยปรับและเงินเพิ่มภาษีอากร 
 5.ขอคัดเอกสารหรือขอสำเนาเอกสาร </t>
+  </si>
+  <si>
+    <t>สามารถทำการยื่นเสียภาษีได้ที่สถานที่ต่อไปนี้เลยค่ะ
+1.สำนักงานสรรพากรทุกสาขาทุกเเห่ง 
+2.ไปรษณีย์ เเบบลงทะเบียน 
+3.ช่องทางออนไลน์ ผ่านเว็บไซต์ของกรมสรรพากร</t>
   </si>
 </sst>
 </file>
@@ -537,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="106" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -604,12 +605,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="25.5">
+    <row r="8" spans="1:2" ht="242.25">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="25.5">
@@ -617,7 +618,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="25.5">
@@ -625,15 +626,15 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="25.5">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="28.5">
-      <c r="A11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.5">
@@ -641,7 +642,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.5">
@@ -649,7 +650,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.5">
@@ -657,7 +658,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="28.5">
@@ -665,15 +666,15 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.5">
       <c r="A16" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="28.5">
@@ -681,7 +682,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="28.5">
@@ -689,7 +690,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="28.5">
@@ -697,7 +698,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.5">
@@ -705,96 +706,99 @@
         <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="28.5">
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="89.25">
-      <c r="A21" s="4" t="s">
+    <row r="22" spans="1:2" ht="89.25">
+      <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="76.5">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:2" ht="76.5">
+      <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="89.25">
-      <c r="A23" s="4" t="s">
+    <row r="24" spans="1:2" ht="89.25">
+      <c r="A24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="76.5">
+      <c r="A25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="127.5">
+      <c r="A26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="102">
+      <c r="A27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="63.75">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="25.5">
+      <c r="A29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="63.75">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="76.5">
-      <c r="A24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="127.5">
-      <c r="A25" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="102">
-      <c r="A26" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="63.75">
-      <c r="A27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="25.5">
-      <c r="A28" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="38.25">
-      <c r="A29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="38.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:2" ht="38.25">
+      <c r="A31" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="242.25">
-      <c r="A31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>45</v>
-      </c>
+    <row r="32" spans="1:2">
+      <c r="B32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add response about time open page
</commit_message>
<xml_diff>
--- a/chat_bot/data/response_law.xlsx
+++ b/chat_bot/data/response_law.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>tag</t>
   </si>
@@ -35,15 +35,6 @@
     <t>greeting</t>
   </si>
   <si>
-    <t>สวัสดี</t>
-  </si>
-  <si>
-    <t>สวัสดีครับ</t>
-  </si>
-  <si>
-    <t>สวัสดีค่ะ</t>
-  </si>
-  <si>
     <t>invite-eating</t>
   </si>
   <si>
@@ -56,9 +47,6 @@
     <t>unknow-message</t>
   </si>
   <si>
-    <t>ไม่เข้าใจคำถาม</t>
-  </si>
-  <si>
     <t>รับประทานแล้วขอบคุณนะคะ</t>
   </si>
   <si>
@@ -80,30 +68,18 @@
     <t>ไม่ได้ทำอะไรค่ะ</t>
   </si>
   <si>
-    <t>ไม่ได้ทำอะไรคับ</t>
-  </si>
-  <si>
-    <t>มีอะไรให้ช่วยไหมครับ</t>
-  </si>
-  <si>
     <t>greeting-inquiries</t>
   </si>
   <si>
     <t>ยินดีให้บริการค่ะ</t>
   </si>
   <si>
-    <t>ท่านต้องการสอบถามด้านใด</t>
-  </si>
-  <si>
     <t>ระบุคำถามได้เลยค่ะ</t>
   </si>
   <si>
     <t>ต้องการข้อมูลด้านใดคะ</t>
   </si>
   <si>
-    <t>ยินดีให้บริการครับ</t>
-  </si>
-  <si>
     <t>quetions-law</t>
   </si>
   <si>
@@ -119,7 +95,42 @@
     <t xml:space="preserve">not-pay </t>
   </si>
   <si>
-    <t>ภาษี สามารแบ่งออกเป็น 5 ประเภทด้วยกันครับ
+    <t>law-why</t>
+  </si>
+  <si>
+    <t>law-calculate</t>
+  </si>
+  <si>
+    <t>law-time</t>
+  </si>
+  <si>
+    <t>law-salary</t>
+  </si>
+  <si>
+    <t>law-place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">สิทธิของประชาชนผู้เสียภาษีมีดังต่อไปนี้
+1.การผ่อนชำระภาษี
+2.การยื่นอุทธรณ์คัดค้านการประเมินภาษี 
+3.ขอทุเลาการชำระภาษีอากรโดยจัดให้มีหลักประกันการชำระหนี้ภาษีอากรค้าง 
+4.ของดหรือลดเบี้ยปรับและเงินเพิ่มภาษีอากร 
+5.ขอคัดเอกสารหรือขอสำเนาเอกสาร </t>
+  </si>
+  <si>
+    <t>สามารถทำการยื่นเสียภาษีได้ที่สถานที่ต่อไปนี้เลยค่ะ
+1.สำนักงานสรรพากรทุกสาขาทุกเเห่ง 
+2.ไปรษณีย์ เเบบลงทะเบียน 
+3.ช่องทางออนไลน์ ผ่านเว็บไซต์ของกรมสรรพากร</t>
+  </si>
+  <si>
+    <t>ท่านต้องการสอบถามด้านใดคะ</t>
+  </si>
+  <si>
+    <t>กฎหมายภาษี เป็นกฎหมายที่บัญญัติขึ้นภายใต้รัฐธรรมนูญ โดยมีจุดประสงค์เพื่อกำหนดควบคุมอัตราการแลกเปลี่ยนเงินในประเทศและเป็นกฎหมายที่ให้อำนาจแก่รัฐในการจัดเก็บภาษีจากราษฎร เพื่อนำไปใช้เป็นประโยชน์ต่อสังคมโดยรวมและผลักดันการพัฒนาเศรษฐกิจของประเทศค่ะ</t>
+  </si>
+  <si>
+    <t>ภาษี สามารแบ่งออกเป็น 5 ประเภทด้วยกันค่ะ
  1.ภาษีบุคคลธรรมดา(PIT)
  2.ภาษีเงินได้นิติบุคคล 
  3.ภาษีมูลค่าเพิ่ม(VAT) 
@@ -127,47 +138,35 @@
  5.อากรแสตมป์(SD)</t>
   </si>
   <si>
-    <t>หากไม่เสียภาษีตามกฎหมายที่กำหนด ตามบทบัญญัติแห่งประมวลกฎหมายรัษฎากร โดยปกติประชาชนทุกคนไม่ว่าจะบุคคลใดจะต้องมีหน้าที่เสียภาษีตามข้อบังคับของกฎหมายรัฐธรรมนูญ และจำเป็นที่จะต้องมีการยื่นแบบการเสียภาษี เพื่อให้ทางรัฐบาลได้รู้ว่าบุคคลมีความบริสุทธิ์ใจที่จะไม่หลีกเลี่ยงการเสียภาษี หากผู้ใดไม่เสียภาษีตามที่กฎหมายกำหนดจะต้องได้รับโทษตามประมวลกฎหมายรัษฎากรและต้องรับผิดทางแพ่งและทางอาญาด้วย</t>
-  </si>
-  <si>
-    <t>กฎหมายภาษี เป็นกฎหมายที่บัญญัติขึ้นภายใต้รัฐธรรมนูญ โดยมีจุดประสงค์เพื่อกำหนดควบคุมอัตราการแลกเปลี่ยนเงินในประเทศและเป็นกฎหมายที่ให้อำนาจแก่รัฐในการจัดเก็บภาษีจากราษฎร เพื่อนำไปใช้เป็นประโยชน์ต่อสังคมโดยรวมและผลักดันการพัฒนาเศรษฐกิจของประเทศครับ</t>
-  </si>
-  <si>
-    <t>หน่วยงานของรัฐสามารถจัดเก็บภาษีอากร แบ่งเป็น 2 ทาง ดังนี้
+    <t>หน่วยงานของรัฐสามารถจัดเก็บภาษีอากร แบ่งเป็น 2 ทาง ดังนี้ค่ะ
 ภาษีทางตรง ได้แก่  ภาษีเงินได้บุคคลธรรมดา ภาษีเงินได้นิติบุคคล 
 ภาษีทางอ้อม ได้แก่ ภาษีมูลค่าเพิ่ม ภาษีธุรกิจเฉพาะ</t>
   </si>
   <si>
-    <t>law-why</t>
-  </si>
-  <si>
-    <t>เพื่อเป็นเครื่องมือส่งเสริมความเจริญเติบโตทางเศรษฐกิจ
- -เพื่อเป็นเครื่องมือในการควบคุมการบริโภคของประชาชนและบำรุงสาธารณูปโภคเละบริการสาธารณะ
- -เพื่อเป็นเครื่องมือในการกระจายรายได้แก่ให้ประชาชนและเป็นการรักษาเสถียรภาพในทางเศรษฐกิจของประเทศ</t>
-  </si>
-  <si>
-    <t>law-calculate</t>
-  </si>
-  <si>
-    <t>การคำนวณภาษีของบุคคลธรรมดา เงินได้สุทธิซึ่งเป็นฐานภาษีสำหรับคำนวณภาษีเงินได้บุคคลธรรมดาซึ่งมาจากเงินได้พึงประเมินที่หักค่าใช้จ่ายและค่าลดหย่อนเรียบร้อยแล้ว (ค่าใช้จ่าย-ค่าลดหย่อน=เงินได้สุทธิ)</t>
-  </si>
-  <si>
-    <t>law-time</t>
-  </si>
-  <si>
-    <t>กฎหมายกำหนดให้บุคคลต้องทำการยื่นเสียภาษีในช่วง 1 มกราคม - 31 มีนาคม ของทุกปี</t>
-  </si>
-  <si>
-    <t>law-salary</t>
-  </si>
-  <si>
-    <t>หากมีเงินเดือนหรือมีรายได้จากหลายทางเกิน 10,000 บาท/เดือน (120,000 บาท/ปี) ต้องยื่นภาษีทุกคน</t>
-  </si>
-  <si>
-    <t>law-place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ขออภัยค่ะ ระบบอัติโนมัติยังไม่เข้าใจคำถามของคุณ หากต้องการสอบถามข้อมูลด้านใดเกี่ยวกับภาษี สามารถถามคำถามดังต่อไปนี้ได้เลยค่ะ
+    <t>หากไม่เสียภาษีตามกฎหมายที่กำหนด ตามบทบัญญัติแห่งประมวลกฎหมายรัษฎากร โดยปกติประชาชนทุกคนไม่ว่าจะบุคคลใดจะต้องมีหน้าที่เสียภาษีตามข้อบังคับของกฎหมายรัฐธรรมนูญ และจำเป็นที่จะต้องมีการยื่นแบบการเสียภาษี เพื่อให้ทางรัฐบาลได้รู้ว่าบุคคลมีความบริสุทธิ์ใจที่จะไม่หลีกเลี่ยงการเสียภาษี หากผู้ใดไม่เสียภาษีตามที่กฎหมายกำหนดจะต้องได้รับโทษตามประมวลกฎหมายรัษฎากรและต้องรับผิดทางแพ่งและทางอาญาด้วยค่ะ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">สวัสดีค่ะ ขอต้อนรับเข้าสู่เพจให้ความรู้ทางกฎหมายของพวกเรา รู้เท่าทันกฎหมายภาษี:Know the tax law ค่ะ </t>
+  </si>
+  <si>
+    <t>time-page</t>
+  </si>
+  <si>
+    <t>1.เพื่อเป็นเครื่องมือส่งเสริมความเจริญเติบโตทางเศรษฐกิจ
+2.เพื่อเป็นเครื่องมือในการควบคุมการบริโภคของประชาชนและบำรุงสาธารณูปโภคเละบริการสาธารณะ
+3.เพื่อเป็นเครื่องมือในการกระจายรายได้แก่ให้ประชาชนและเป็นการรักษาเสถียรภาพในทางเศรษฐกิจของประเทศ</t>
+  </si>
+  <si>
+    <t>การคำนวณภาษีของบุคคลธรรมดานะคะ จากเงินได้สุทธิซึ่งเป็นฐานภาษีสำหรับคำนวณภาษีเงินได้บุคคลธรรมดา ซึ่งมาจากเงินได้พึงประเมินที่หักค่าใช้จ่ายและค่าลดหย่อนเรียบร้อยแล้ว (ค่าใช้จ่าย-ค่าลดหย่อน=เงินได้สุทธิ)</t>
+  </si>
+  <si>
+    <t>กฎหมายกำหนดให้บุคคลต้องทำการยื่นเสียภาษีในช่วง 1 มกราคม - 31 มีนาคม ของทุกปีค่ะ</t>
+  </si>
+  <si>
+    <t>หากมีเงินเดือนหรือมีรายได้จากหลายทางเกิน 10,000 บาท/เดือน (120,000 บาท/ปี) ต้องยื่นภาษีทุกคนค่ะ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ขออภัยค่ะ บอทยังไม่เข้าใจคำถามของคุณ หากต้องการสอบถามข้อมูลด้านใดเกี่ยวกับภาษี สามารถถามคำถามดังต่อไปนี้ได้เลยค่ะ
 1.กฎหมายภาษืคืออะไร
 2.ภาษีมีกี่ประเภท
 3.สิทธิของประชาชนผู้เสียภาษีมีอะไรบ้าง
@@ -180,18 +179,8 @@
 10.บุคคลธรรมดาต้องมีเงินเดือนเท่าไร ถึงต้องยื่นภาษี </t>
   </si>
   <si>
-    <t xml:space="preserve">สิทธิของประชาชนผู้เสียภาษีมีดังต่อไปนี้
-1.การผ่อนชำระภาษี
-2.การยื่นอุทธรณ์คัดค้านการประเมินภาษี 
-3.ขอทุเลาการชำระภาษีอากรโดยจัดให้มีหลักประกันการชำระหนี้ภาษีอากรค้าง 
-4.ของดหรือลดเบี้ยปรับและเงินเพิ่มภาษีอากร 
-5.ขอคัดเอกสารหรือขอสำเนาเอกสาร </t>
-  </si>
-  <si>
-    <t>สามารถทำการยื่นเสียภาษีได้ที่สถานที่ต่อไปนี้เลยค่ะ
-1.สำนักงานสรรพากรทุกสาขาทุกเเห่ง 
-2.ไปรษณีย์ เเบบลงทะเบียน 
-3.ช่องทางออนไลน์ ผ่านเว็บไซต์ของกรมสรรพากร</t>
+    <t>เวลาเปิดทำการของเพจมีช่วงเวลา ดังนี้เลยค่ะ
+จันทร์-ศุกร์ เวลา 9.00-17.00 น.</t>
   </si>
 </sst>
 </file>
@@ -540,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="106" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -557,25 +546,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="38.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="25.5">
+      <c r="A3" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="25.5">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -583,66 +572,66 @@
     </row>
     <row r="5" spans="1:2" ht="25.5">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="25.5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="242.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="242.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="25.5">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="25.5">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="28.5">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="25.5">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row r="11" spans="1:2" ht="28.5">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="25.5">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.5">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.5">
@@ -650,7 +639,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.5">
@@ -658,7 +647,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="28.5">
@@ -666,7 +655,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.5">
@@ -674,127 +663,87 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="89.25">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="76.5">
+      <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="28.5">
-      <c r="A17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="28.5">
-      <c r="A18" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="28.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="89.25">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="76.5">
+      <c r="A20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="127.5">
+      <c r="A21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="102">
+      <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="28.5">
-      <c r="A20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="63.75">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="28.5">
-      <c r="A21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="B23" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="25.5">
+      <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="89.25">
-      <c r="A22" s="4" t="s">
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="63.75">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="38.25">
+      <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="76.5">
-      <c r="A23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="89.25">
-      <c r="A24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="76.5">
-      <c r="A25" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="127.5">
-      <c r="A26" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="B26" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="102">
-      <c r="A27" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="63.75">
-      <c r="A28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="25.5">
-      <c r="A29" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="3" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="63.75">
-      <c r="A30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="38.25">
-      <c r="A31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:2">

</xml_diff>

<commit_message>
add response and train for thankyou
</commit_message>
<xml_diff>
--- a/chat_bot/data/response_law.xlsx
+++ b/chat_bot/data/response_law.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>tag</t>
   </si>
@@ -181,6 +181,12 @@
   <si>
     <t>เวลาเปิดทำการของเพจมีช่วงเวลา ดังนี้เลยค่ะ
 จันทร์-ศุกร์ เวลา 9.00-17.00 น.</t>
+  </si>
+  <si>
+    <t>thank-you</t>
+  </si>
+  <si>
+    <t>ยินดีค่ะ ขอบคุณที่ใช้บริการกับเพจเรานะคะ โอกาสหน้าเชิญใหม่ค่ะ</t>
   </si>
 </sst>
 </file>
@@ -529,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="106" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -746,6 +752,14 @@
         <v>40</v>
       </c>
     </row>
+    <row r="27" spans="1:2" ht="25.5">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="32" spans="1:2">
       <c r="B32" s="3"/>
     </row>

</xml_diff>

<commit_message>
add question and response about image
</commit_message>
<xml_diff>
--- a/chat_bot/data/response_law.xlsx
+++ b/chat_bot/data/response_law.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>tag</t>
   </si>
@@ -188,12 +188,18 @@
   <si>
     <t>ยินดีค่ะ ขอบคุณที่ใช้บริการกับเพจเรานะคะ โอกาสหน้าเชิญใหม่ค่ะ</t>
   </si>
+  <si>
+    <t>test-image</t>
+  </si>
+  <si>
+    <t>https://static.trueplookpanya.com/tppy/member/m_685000_687500/686480/cms/images/81unMcmp3RL._SX450_.jpg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +226,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -238,10 +252,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -253,8 +268,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="106" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -752,16 +771,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="25.5">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="25.5">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="B32" s="3"/>
+    <row r="31" spans="1:2">
+      <c r="B31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add question and respon for bot send image
</commit_message>
<xml_diff>
--- a/chat_bot/data/response_law.xlsx
+++ b/chat_bot/data/response_law.xlsx
@@ -189,10 +189,10 @@
     <t>ยินดีค่ะ ขอบคุณที่ใช้บริการกับเพจเรานะคะ โอกาสหน้าเชิญใหม่ค่ะ</t>
   </si>
   <si>
-    <t>test-image</t>
-  </si>
-  <si>
-    <t>https://static.trueplookpanya.com/tppy/member/m_685000_687500/686480/cms/images/81unMcmp3RL._SX450_.jpg</t>
+    <t>law-pay</t>
+  </si>
+  <si>
+    <t>https://obs.line-scdn.net/0hhlVJ2T8yN0NrMxuamsZIFFFlNCxYXyRADwVmQDddaXcWUCRCBQV7dkc6bnZBAXAdAlRwLUsyLHJAVCMWVV17/w644</t>
   </si>
 </sst>
 </file>
@@ -552,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="106" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="106" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -771,27 +771,30 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" ht="25.5">
       <c r="A27" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="25.5">
+      <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="71.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="B31" s="3"/>
+      <c r="B28" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="B30" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B28" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>